<commit_message>
Complete part 1 of 1c
</commit_message>
<xml_diff>
--- a/assignment_1d/wind_turbine_linear_programming_analysis.xlsx
+++ b/assignment_1d/wind_turbine_linear_programming_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Projects\git\design-optimisation\assignment_1d\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA9DEA8-4DB9-49FA-BC6B-A72EC67A4640}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA57E3C-D83F-4350-8C0D-AFC91EB12D75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,17 +21,17 @@
     <definedName name="investment_available">'Provided Data'!$E$25</definedName>
     <definedName name="plot_length_available">'Provided Data'!$C$33:$E$33</definedName>
     <definedName name="plot_length_required">'Provided Data'!$C$29:$E$29</definedName>
-    <definedName name="solver_adj" localSheetId="1" hidden="1">'Quantity Calculation'!$D$20:$F$22</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">'Quantity Calculation'!$D$19:$F$21</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="1" hidden="1">'Quantity Calculation'!$D$20:$F$22</definedName>
-    <definedName name="solver_lhs2" localSheetId="1" hidden="1">'Quantity Calculation'!$D$33</definedName>
-    <definedName name="solver_lhs3" localSheetId="1" hidden="1">'Quantity Calculation'!$E$33</definedName>
-    <definedName name="solver_lhs4" localSheetId="1" hidden="1">'Quantity Calculation'!$F$33</definedName>
-    <definedName name="solver_lhs5" localSheetId="1" hidden="1">'Quantity Calculation'!$H$36</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">'Quantity Calculation'!$D$19:$F$21</definedName>
+    <definedName name="solver_lhs2" localSheetId="1" hidden="1">'Quantity Calculation'!$D$32</definedName>
+    <definedName name="solver_lhs3" localSheetId="1" hidden="1">'Quantity Calculation'!$E$32</definedName>
+    <definedName name="solver_lhs4" localSheetId="1" hidden="1">'Quantity Calculation'!$F$32</definedName>
+    <definedName name="solver_lhs5" localSheetId="1" hidden="1">'Quantity Calculation'!$H$35</definedName>
     <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
@@ -40,7 +40,7 @@
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">5</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="1" hidden="1">'Quantity Calculation'!$L$28</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">'Quantity Calculation'!$L$27</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">4</definedName>
@@ -224,9 +224,6 @@
     <t>ROI</t>
   </si>
   <si>
-    <t>Use Initial Investment Before</t>
-  </si>
-  <si>
     <t>If true, initial investment will be considered before calculating optimal turbine numbers</t>
   </si>
   <si>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>Total Turbine Investment</t>
+  </si>
+  <si>
+    <t>Use Initial Investment</t>
   </si>
 </sst>
 </file>
@@ -243,7 +243,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,6 +268,14 @@
     </font>
     <font>
       <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -344,7 +352,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -358,12 +366,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -372,26 +374,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -401,30 +385,66 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -710,33 +730,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="4">
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="23">
         <v>1</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="23">
         <v>2</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="23">
         <v>3</v>
       </c>
     </row>
@@ -744,46 +764,46 @@
       <c r="B4" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="22">
         <v>2</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="5">
         <v>32</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="26"/>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="22">
         <v>6</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="22">
         <v>4</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F5" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="26"/>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="25">
-        <v>0</v>
-      </c>
-      <c r="E6" s="25">
-        <v>0</v>
-      </c>
-      <c r="F6" s="25">
+      <c r="D6" s="22">
+        <v>0</v>
+      </c>
+      <c r="E6" s="22">
+        <v>0</v>
+      </c>
+      <c r="F6" s="22">
         <v>3</v>
       </c>
     </row>
@@ -799,10 +819,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FAE770D-E143-46BB-93B8-0BA442FD6E70}">
-  <dimension ref="B2:M37"/>
+  <dimension ref="B2:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,10 +837,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="18"/>
+      <c r="C2" s="30"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C3">
@@ -828,19 +848,19 @@
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="7" t="s">
+      <c r="C5" s="29"/>
+      <c r="D5" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
       <c r="D6" t="s">
         <v>24</v>
       </c>
@@ -850,11 +870,11 @@
       <c r="F6" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
+      <c r="H6" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
@@ -863,38 +883,38 @@
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="13">
         <f>- 'Provided Data'!C$13 - 'Provided Data'!C$20</f>
         <v>-300324</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="13">
         <f xml:space="preserve"> - 'Provided Data'!F$13 - 'Provided Data'!F$20</f>
         <v>-2787600</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="13">
         <f xml:space="preserve"> - 'Provided Data'!I$13 - 'Provided Data'!I$20</f>
         <v>-4475900</v>
       </c>
-      <c r="H7" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
+      <c r="H7" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="26"/>
       <c r="C8">
         <v>2</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="13">
         <f>- 'Provided Data'!D$13 - 'Provided Data'!D$20</f>
         <v>-1032240</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="13">
         <f xml:space="preserve"> - 'Provided Data'!G$13 - 'Provided Data'!G$20</f>
         <v>-5019225</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="13">
         <f xml:space="preserve"> - 'Provided Data'!J$13 - 'Provided Data'!J$20</f>
         <v>-9672600</v>
       </c>
@@ -904,41 +924,41 @@
       <c r="C9">
         <v>3</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="13">
         <f xml:space="preserve"> - 'Provided Data'!E$13 - 'Provided Data'!E$20</f>
         <v>-4798800</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="13">
         <f xml:space="preserve"> - 'Provided Data'!H$13 - 'Provided Data'!H$20</f>
         <v>-6973375</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F9" s="13">
         <f xml:space="preserve"> - 'Provided Data'!K$13 - 'Provided Data'!K$20</f>
         <v>-9769600</v>
       </c>
       <c r="H9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="7" t="s">
+      <c r="C11" s="29"/>
+      <c r="D11" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
       <c r="D12" t="s">
         <v>24</v>
       </c>
@@ -956,15 +976,15 @@
       <c r="C13">
         <v>1</v>
       </c>
-      <c r="D13" s="21">
+      <c r="D13" s="13">
         <f>$C$3* 'Provided Data'!C$6+D7*$H$7</f>
         <v>2919000</v>
       </c>
-      <c r="E13" s="21">
+      <c r="E13" s="13">
         <f>$C$3* 'Provided Data'!F$6+E7*$H$7</f>
         <v>4843800</v>
       </c>
-      <c r="F13" s="21">
+      <c r="F13" s="13">
         <f>$C$3* 'Provided Data'!I$6+F7*$H$7</f>
         <v>5285500</v>
       </c>
@@ -974,15 +994,15 @@
       <c r="C14">
         <v>2</v>
       </c>
-      <c r="D14" s="21">
+      <c r="D14" s="13">
         <f>$C$3* 'Provided Data'!D$6+D8*$H$7</f>
         <v>6348000</v>
       </c>
-      <c r="E14" s="21">
+      <c r="E14" s="13">
         <f>$C$3* 'Provided Data'!G$6+E8*$H$7</f>
         <v>8648000</v>
       </c>
-      <c r="F14" s="21">
+      <c r="F14" s="13">
         <f>$C$3* 'Provided Data'!J$6+F8*$H$7</f>
         <v>11728800</v>
       </c>
@@ -992,411 +1012,405 @@
       <c r="C15">
         <v>3</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="13">
         <f>$C$3* 'Provided Data'!E$6+D9*$H$7</f>
         <v>5592000</v>
       </c>
-      <c r="E15" s="21">
+      <c r="E15" s="13">
         <f>$C$3* 'Provided Data'!H$6+E9*$H$7</f>
         <v>965080</v>
       </c>
-      <c r="F15" s="21">
+      <c r="F15" s="13">
         <f>$C$3* 'Provided Data'!K$6+F9*$H$7</f>
         <v>28200000</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="23"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
+      <c r="B16" s="15"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="23"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
+      <c r="B17" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="29"/>
+      <c r="D17" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="H17" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="I17" s="29"/>
+      <c r="J17" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="K17" s="25"/>
+      <c r="L17" s="25"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" t="s">
+        <v>24</v>
+      </c>
+      <c r="K18" t="s">
+        <v>25</v>
+      </c>
+      <c r="L18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B19" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" s="17">
+        <v>2</v>
+      </c>
+      <c r="E19" s="17">
+        <v>6</v>
+      </c>
+      <c r="F19" s="17">
+        <v>0</v>
+      </c>
+      <c r="H19" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19" s="13">
+        <f t="shared" ref="J19:L21" si="0">D7*D19</f>
+        <v>-600648</v>
+      </c>
+      <c r="K19" s="13">
+        <f t="shared" si="0"/>
+        <v>-16725600</v>
+      </c>
+      <c r="L19" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B20" s="26"/>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20" s="17">
         <v>32</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="H18" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="I18" s="20"/>
-      <c r="J18" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" t="s">
-        <v>24</v>
-      </c>
-      <c r="E19" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" t="s">
-        <v>26</v>
-      </c>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" t="s">
-        <v>24</v>
-      </c>
-      <c r="K19" t="s">
-        <v>25</v>
-      </c>
-      <c r="L19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20" s="25">
+      <c r="E20" s="17">
+        <v>4</v>
+      </c>
+      <c r="F20" s="17">
+        <v>0</v>
+      </c>
+      <c r="H20" s="26"/>
+      <c r="I20">
         <v>2</v>
       </c>
-      <c r="E20" s="25">
-        <v>6</v>
-      </c>
-      <c r="F20" s="25">
-        <v>0</v>
-      </c>
-      <c r="H20" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="I20">
-        <v>1</v>
-      </c>
-      <c r="J20" s="21">
-        <f>D7*D20</f>
-        <v>-600648</v>
-      </c>
-      <c r="K20" s="21">
-        <f t="shared" ref="K20:L22" si="0">E7*E20</f>
-        <v>-16725600</v>
-      </c>
-      <c r="L20" s="21">
+      <c r="J20" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-33031680</v>
+      </c>
+      <c r="K20" s="13">
+        <f t="shared" si="0"/>
+        <v>-20076900</v>
+      </c>
+      <c r="L20" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="26"/>
       <c r="C21">
-        <v>2</v>
-      </c>
-      <c r="D21" s="25">
-        <v>32</v>
-      </c>
-      <c r="E21" s="25">
-        <v>4</v>
-      </c>
-      <c r="F21" s="25">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D21" s="17">
+        <v>0</v>
+      </c>
+      <c r="E21" s="17">
+        <v>0</v>
+      </c>
+      <c r="F21" s="17">
+        <v>3</v>
       </c>
       <c r="H21" s="26"/>
       <c r="I21">
-        <v>2</v>
-      </c>
-      <c r="J21" s="21">
-        <f t="shared" ref="J21:J22" si="1">D8*D21</f>
-        <v>-33031680</v>
-      </c>
-      <c r="K21" s="21">
+        <v>3</v>
+      </c>
+      <c r="J21" s="13">
         <f t="shared" si="0"/>
-        <v>-20076900</v>
-      </c>
-      <c r="L21" s="21">
+        <v>0</v>
+      </c>
+      <c r="K21" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M21" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="26"/>
-      <c r="C22">
-        <v>3</v>
-      </c>
-      <c r="D22" s="25">
-        <v>0</v>
-      </c>
-      <c r="E22" s="25">
-        <v>0</v>
-      </c>
-      <c r="F22" s="25">
-        <v>3</v>
-      </c>
-      <c r="H22" s="26"/>
-      <c r="I22">
-        <v>3</v>
-      </c>
-      <c r="J22" s="21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K22" s="21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L22" s="21">
+      <c r="L21" s="13">
         <f t="shared" si="0"/>
         <v>-29308800</v>
       </c>
-      <c r="M22" s="21">
-        <f>SUM(J20:L22)</f>
+      <c r="M21" s="13">
+        <f>SUM(J19:L21)</f>
         <v>-99743628</v>
       </c>
     </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+    </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
+      <c r="B23" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="29"/>
+      <c r="D23" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
-      <c r="D25" t="s">
-        <v>24</v>
-      </c>
-      <c r="E25" t="s">
-        <v>25</v>
-      </c>
-      <c r="F25" t="s">
-        <v>26</v>
+      <c r="B25" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" s="13">
+        <f t="shared" ref="D25:F27" si="1">D13*D19</f>
+        <v>5838000</v>
+      </c>
+      <c r="E25" s="13">
+        <f t="shared" si="1"/>
+        <v>29062800</v>
+      </c>
+      <c r="F25" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B26" s="26" t="s">
-        <v>12</v>
-      </c>
+      <c r="B26" s="26"/>
       <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26" s="21">
-        <f>D13*D20</f>
-        <v>5838000</v>
-      </c>
-      <c r="E26" s="21">
-        <f t="shared" ref="E26:F26" si="2">E13*E20</f>
-        <v>29062800</v>
-      </c>
-      <c r="F26" s="21">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="D26" s="13">
+        <f t="shared" si="1"/>
+        <v>203136000</v>
+      </c>
+      <c r="E26" s="13">
+        <f t="shared" si="1"/>
+        <v>34592000</v>
+      </c>
+      <c r="F26" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" s="26"/>
       <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E27" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="13">
+        <f t="shared" si="1"/>
+        <v>84600000</v>
+      </c>
+      <c r="G27" s="13">
+        <f>SUM(D25:F27)</f>
+        <v>357228800</v>
+      </c>
+      <c r="H27" s="16">
+        <f>(G27+M21)/-M21</f>
+        <v>2.5814698859760745</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B28" s="21"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B29" s="21"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C30" s="18"/>
+      <c r="D30" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B31" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="32"/>
+      <c r="D31" cm="1">
+        <f t="array" ref="D31">SUMPRODUCT(TRANSPOSE(D19:D21), plot_length_required)</f>
+        <v>5000</v>
+      </c>
+      <c r="E31" cm="1">
+        <f t="array" ref="E31">SUMPRODUCT(TRANSPOSE(E19:E21), plot_length_required)</f>
+        <v>1200</v>
+      </c>
+      <c r="F31" cm="1">
+        <f t="array" ref="F31">SUMPRODUCT(TRANSPOSE(F19:F21), plot_length_required)</f>
+        <v>750</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B32" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="32"/>
+      <c r="D32">
+        <f>'Provided Data'!C33-D31</f>
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <f>'Provided Data'!D33-E31</f>
+        <v>8800</v>
+      </c>
+      <c r="F32">
+        <f>'Provided Data'!E33-F31</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C34" s="18"/>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
         <v>2</v>
       </c>
-      <c r="D27" s="21">
-        <f t="shared" ref="D27:F27" si="3">D14*D21</f>
-        <v>203136000</v>
-      </c>
-      <c r="E27" s="21">
-        <f t="shared" si="3"/>
-        <v>34592000</v>
-      </c>
-      <c r="F27" s="21">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G27" s="1" t="s">
+      <c r="F34">
+        <v>3</v>
+      </c>
+      <c r="G34" t="s">
         <v>31</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="26"/>
-      <c r="C28">
-        <v>3</v>
-      </c>
-      <c r="D28" s="21">
-        <f t="shared" ref="D28:F28" si="4">D15*D22</f>
-        <v>0</v>
-      </c>
-      <c r="E28" s="21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F28" s="21">
-        <f t="shared" si="4"/>
-        <v>84600000</v>
-      </c>
-      <c r="G28" s="21">
-        <f>IF(H7, SUM(D26:F28), SUM(D26:F28)+M22)</f>
-        <v>257485172</v>
-      </c>
-      <c r="H28" s="24">
-        <f>G28/investment_available</f>
-        <v>2.5748517199999998</v>
-      </c>
-    </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B29" s="34"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B30" s="34"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-    </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C31" s="27"/>
-      <c r="D31" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="E31" t="s">
-        <v>25</v>
-      </c>
-      <c r="F31" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B32" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="C32" s="30"/>
-      <c r="D32" cm="1">
-        <f t="array" ref="D32">SUMPRODUCT(TRANSPOSE(D20:D22), plot_length_required)</f>
-        <v>5000</v>
-      </c>
-      <c r="E32" cm="1">
-        <f t="array" ref="E32">SUMPRODUCT(TRANSPOSE(E20:E22), plot_length_required)</f>
-        <v>1200</v>
-      </c>
-      <c r="F32" cm="1">
-        <f t="array" ref="F32">SUMPRODUCT(TRANSPOSE(F20:F22), plot_length_required)</f>
-        <v>750</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C33" s="30"/>
-      <c r="D33">
-        <f>'Provided Data'!C33-D32</f>
-        <v>0</v>
-      </c>
-      <c r="E33">
-        <f>'Provided Data'!D33-E32</f>
-        <v>8800</v>
-      </c>
-      <c r="F33">
-        <f>'Provided Data'!E33-F32</f>
-        <v>0</v>
+      <c r="H34" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C35" s="27"/>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35">
-        <v>2</v>
-      </c>
-      <c r="F35">
-        <v>3</v>
-      </c>
-      <c r="G35" t="s">
-        <v>31</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>34</v>
+      <c r="B35" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="34"/>
+      <c r="D35" s="3">
+        <f>-SUMPRODUCT(D7:D9,D19:D21)</f>
+        <v>33632328</v>
+      </c>
+      <c r="E35" s="3">
+        <f>-SUMPRODUCT(E7:E9,E19:E21)</f>
+        <v>36802500</v>
+      </c>
+      <c r="F35" s="3">
+        <f>-SUMPRODUCT(F7:F9,F19:F21)</f>
+        <v>29308800</v>
+      </c>
+      <c r="G35" s="13">
+        <f>SUM(D35:F35)</f>
+        <v>99743628</v>
+      </c>
+      <c r="H35" s="20">
+        <f>investment_available-G35</f>
+        <v>256372</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="C36" s="32"/>
-      <c r="D36" s="3">
-        <f>-SUMPRODUCT(D7:D9,D20:D22)</f>
-        <v>33632328</v>
-      </c>
-      <c r="E36" s="3">
-        <f>-SUMPRODUCT(E7:E9,E20:E22)</f>
-        <v>36802500</v>
-      </c>
-      <c r="F36" s="3">
-        <f>-SUMPRODUCT(F7:F9,F20:F22)</f>
-        <v>29308800</v>
-      </c>
-      <c r="G36" s="21">
-        <f>SUM(D36:F36)</f>
-        <v>99743628</v>
-      </c>
-      <c r="H36" s="33">
-        <f>investment_available-G36</f>
-        <v>256372</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="28"/>
-      <c r="C37" s="28"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B11:C12"/>
+    <mergeCell ref="B17:C18"/>
+    <mergeCell ref="B19:B21"/>
     <mergeCell ref="H6:J6"/>
     <mergeCell ref="H7:J7"/>
-    <mergeCell ref="B24:C25"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="H18:I19"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="B23:C24"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="H17:I18"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="H19:H21"/>
     <mergeCell ref="B5:C6"/>
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B13:B15"/>
     <mergeCell ref="D11:F11"/>
-    <mergeCell ref="B11:C12"/>
-    <mergeCell ref="B18:C19"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D17:F17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1407,7 +1421,7 @@
   <dimension ref="B2:N34"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1418,49 +1432,49 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="15"/>
-      <c r="C4" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="8" t="s">
+      <c r="B4" s="12"/>
+      <c r="C4" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="25"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="8" t="s">
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="7" t="s">
         <v>3</v>
       </c>
       <c r="G5" s="6" t="s">
@@ -1469,7 +1483,7 @@
       <c r="H5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="7" t="s">
         <v>3</v>
       </c>
       <c r="J5" s="6" t="s">
@@ -1486,31 +1500,31 @@
       <c r="B6" s="2">
         <v>13</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="8">
         <v>145950</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="9">
         <v>317400</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="11">
         <v>279600</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="8">
         <v>242190</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="9">
         <v>432400</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="9">
         <v>48254</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="8">
         <v>264275</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="9">
         <v>586440</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6" s="9">
         <v>1410000</v>
       </c>
       <c r="N6" t="s">
@@ -1528,37 +1542,37 @@
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
       <c r="N10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="15"/>
-      <c r="C11" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="8" t="s">
+      <c r="B11" s="12"/>
+      <c r="C11" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="25"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="8" t="s">
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
       <c r="N11" t="s">
         <v>15</v>
       </c>
@@ -1567,16 +1581,16 @@
       <c r="B12" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="7" t="s">
         <v>3</v>
       </c>
       <c r="G12" s="6" t="s">
@@ -1585,7 +1599,7 @@
       <c r="H12" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="9" t="s">
+      <c r="I12" s="7" t="s">
         <v>3</v>
       </c>
       <c r="J12" s="6" t="s">
@@ -1599,31 +1613,31 @@
       <c r="B13" s="2">
         <v>13</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="8">
         <v>80524</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="9">
         <v>347490</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="11">
         <v>3501300</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="8">
         <v>2497500</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="9">
         <v>3951600</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13" s="9">
         <v>5194000</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13" s="8">
         <v>4003400</v>
       </c>
-      <c r="J13" s="11">
+      <c r="J13" s="9">
         <v>4527600</v>
       </c>
-      <c r="K13" s="11">
+      <c r="K13" s="9">
         <v>7154400</v>
       </c>
       <c r="N13" t="s">
@@ -1636,37 +1650,37 @@
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="F16" s="16" t="s">
+      <c r="F16" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
       <c r="N17" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="15"/>
-      <c r="C18" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="8" t="s">
+      <c r="B18" s="12"/>
+      <c r="C18" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="25"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="8" t="s">
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="25"/>
       <c r="N18" t="s">
         <v>28</v>
       </c>
@@ -1675,16 +1689,16 @@
       <c r="B19" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F19" s="7" t="s">
         <v>3</v>
       </c>
       <c r="G19" s="6" t="s">
@@ -1693,7 +1707,7 @@
       <c r="H19" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I19" s="9" t="s">
+      <c r="I19" s="7" t="s">
         <v>3</v>
       </c>
       <c r="J19" s="6" t="s">
@@ -1707,61 +1721,61 @@
       <c r="B20" s="2">
         <v>13</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="8">
         <v>219800</v>
       </c>
-      <c r="D20" s="11">
+      <c r="D20" s="9">
         <v>684750</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="11">
         <v>1297500</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F20" s="8">
         <v>290100</v>
       </c>
-      <c r="G20" s="11">
+      <c r="G20" s="9">
         <v>1067625</v>
       </c>
-      <c r="H20" s="11">
+      <c r="H20" s="9">
         <v>1779375</v>
       </c>
-      <c r="I20" s="10">
+      <c r="I20" s="8">
         <v>472500</v>
       </c>
-      <c r="J20" s="11">
+      <c r="J20" s="9">
         <v>5145000</v>
       </c>
-      <c r="K20" s="11">
+      <c r="K20" s="9">
         <v>2615200</v>
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="5"/>
+      <c r="D25" s="39"/>
       <c r="E25" s="3">
         <v>100000000</v>
       </c>
     </row>
     <row r="27" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
     </row>
     <row r="28" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
@@ -1786,11 +1800,11 @@
       </c>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C31" s="17" t="s">
+      <c r="C31" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="35"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
@@ -1817,22 +1831,22 @@
     <row r="34" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="F16:H17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F2:H3"/>
+    <mergeCell ref="F9:H10"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="I11:K11"/>
     <mergeCell ref="I18:K18"/>
     <mergeCell ref="C23:E24"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="F4:H4"/>
     <mergeCell ref="I4:K4"/>
-    <mergeCell ref="F2:H3"/>
-    <mergeCell ref="F9:H10"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="F16:H17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="F18:H18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>